<commit_message>
commit sauvegarde 21/09/2021 exploitable en prod
</commit_message>
<xml_diff>
--- a/public/uploads/BENEFICIAIRE_PERSONNE_MORALE.xlsx
+++ b/public/uploads/BENEFICIAIRE_PERSONNE_MORALE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\dekra\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3915EFE-E9FE-45E5-9AA7-CEF11B8A4469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B03F520-A02A-4649-869A-CE203B11DD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28755" yWindow="7935" windowWidth="28680" windowHeight="7335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
   <si>
     <t>RAISON SOCIALE 
  du demandeur</t>
@@ -458,6 +458,15 @@
   </si>
   <si>
     <t>974</t>
+  </si>
+  <si>
+    <t>Surface déclarée dans l'AH/facture (m2)</t>
+  </si>
+  <si>
+    <t>Type d'isolant (soufflé/posé/autre) déclaré</t>
+  </si>
+  <si>
+    <t>Marque et référence de l'isolant déclarées</t>
   </si>
 </sst>
 </file>
@@ -789,20 +798,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AI5" sqref="AI5"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="31" max="36" width="23.140625" customWidth="1"/>
+    <col min="34" max="39" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,26 +902,35 @@
       <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -943,12 +961,15 @@
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
       <c r="AH2" s="5"/>
-      <c r="AI2" s="10"/>
+      <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>